<commit_message>
Adding properties to folders
</commit_message>
<xml_diff>
--- a/Proyecto/Junior - UNO/ConfigFile.xlsx
+++ b/Proyecto/Junior - UNO/ConfigFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan_\OneDrive\Documentos\Power Automate\Repo\Template\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan_\OneDrive\Documentos\Power Automate\Repo\Proyecto\Junior - UNO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047105FE-FC81-466A-B96E-0A337395F702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0533F10-EF1F-46AD-8DEB-DA463BA04556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B7997D2D-BBFB-4006-AE83-D5D951781D58}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B7997D2D-BBFB-4006-AE83-D5D951781D58}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -77,6 +77,21 @@
   </si>
   <si>
     <t>Where we can locate the project in the local workstation (or server)</t>
+  </si>
+  <si>
+    <t>URL_Test</t>
+  </si>
+  <si>
+    <t>https://forms.office.com/Pages/ResponsePage.aspx?id=x8fjOlHq3kaVQBL0EQ6smyFnQk63wvpEhjCaoYxMrW5UQlpSVFVGSlpRWE8xQzFVTEVBMzdZVzRaTC4u</t>
+  </si>
+  <si>
+    <t>C:\Users\ivan_\OneDrive\Documentos\Power Automate\Repo\Proyecto\Junior - UNO</t>
+  </si>
+  <si>
+    <t>C:\Users\ivan_\OneDrive\Documentos\Power Automate\Repo\Proyecto\Junior - UNO\Output\LogFile</t>
+  </si>
+  <si>
+    <t>C:\Users\ivan_\OneDrive\Documentos\Power Automate\Repo\Proyecto\Junior - UNO\Output\ScreenshotError</t>
   </si>
 </sst>
 </file>
@@ -493,18 +508,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA6AD96-B69F-45B6-89C7-E507F4856D36}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="72.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="72.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -515,7 +530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
     </row>
   </sheetData>
@@ -528,17 +543,17 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="80.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="130.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -560,7 +575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -571,33 +586,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
     </row>
   </sheetData>
@@ -609,17 +640,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29154BD-E643-4816-BF02-C077ED023206}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="18.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="76.28515625" style="5" customWidth="1"/>
+    <col min="1" max="2" width="18.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="76.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Finishing to config the Logging Process
</commit_message>
<xml_diff>
--- a/Proyecto/Junior - UNO/ConfigFile.xlsx
+++ b/Proyecto/Junior - UNO/ConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan_\OneDrive\Documentos\Power Automate\Repo\Proyecto\Junior - UNO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0533F10-EF1F-46AD-8DEB-DA463BA04556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E22E2F-2A26-4F88-85B1-9319F30117B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B7997D2D-BBFB-4006-AE83-D5D951781D58}"/>
   </bookViews>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07256ECB-87CF-419B-82BC-C5909F33B71E}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,7 +569,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Adding information about the error handling and finding new errors
</commit_message>
<xml_diff>
--- a/Proyecto/Junior - UNO/ConfigFile.xlsx
+++ b/Proyecto/Junior - UNO/ConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan_\OneDrive\Documentos\Power Automate\Repo\Proyecto\Junior - UNO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E22E2F-2A26-4F88-85B1-9319F30117B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B6D0CA-6204-4F41-BB28-5A0824657F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B7997D2D-BBFB-4006-AE83-D5D951781D58}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>C:\Users\ivan_\OneDrive\Documentos\Power Automate\Repo\Proyecto\Junior - UNO\Output\ScreenshotError</t>
+  </si>
+  <si>
+    <t>SendLogFile</t>
+  </si>
+  <si>
+    <t>ivan_hds11@hotmail.com</t>
+  </si>
+  <si>
+    <t>Correo a donde van a ir todos los Log File generados despues de cada ejecución.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -172,6 +181,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,14 +552,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07256ECB-87CF-419B-82BC-C5909F33B71E}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="130.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" style="2" customWidth="1"/>
     <col min="3" max="3" width="80.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -627,7 +637,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
     </row>

</xml_diff>

<commit_message>
Finishing the OnError label and undertanding the power of error block
</commit_message>
<xml_diff>
--- a/Proyecto/Junior - UNO/ConfigFile.xlsx
+++ b/Proyecto/Junior - UNO/ConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan_\OneDrive\Documentos\Power Automate\Repo\Proyecto\Junior - UNO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B6D0CA-6204-4F41-BB28-5A0824657F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CF372D-D5D9-4670-B0F7-6F7903A0173A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B7997D2D-BBFB-4006-AE83-D5D951781D58}"/>
   </bookViews>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -181,7 +181,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,13 +552,13 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="133.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="80.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -641,7 +640,7 @@
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="5" t="s">

</xml_diff>